<commit_message>
Replaced all <PQL values
</commit_message>
<xml_diff>
--- a/Database/PQL.xlsx
+++ b/Database/PQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/94c7e948e3256fed/AU/Heavy metals in Minas Gerais' soils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basecamp/DataspellProjects/Minas_Gerais/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{4DB8C5D5-50AE-467F-BFA2-9B371C63C774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35DD75D4-E391-4E98-B83F-C40AD13D82ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8CECC2-B00C-B449-B09D-A37747F55FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28060" windowHeight="16360" tabRatio="745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PQL" sheetId="29" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Elemento</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Al</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Ag</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>PQL calculated by Gabriel Franci for samples analyzed in 2013</t>
+  </si>
+  <si>
+    <t>UFV1</t>
   </si>
 </sst>
 </file>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -297,22 +297,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -333,7 +321,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -653,38 +641,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="162" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A36" sqref="A35:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="14"/>
-    <col min="10" max="10" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="9.1640625" style="4"/>
+    <col min="10" max="10" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
-      <c r="B1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>2</v>
@@ -696,30 +683,24 @@
         <v>4</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>10.039999999999999</v>
@@ -727,19 +708,13 @@
       <c r="F3" s="3">
         <v>45.123472628766685</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="15">
         <v>3.1288243555515738</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>0.43</v>
@@ -756,19 +731,13 @@
       <c r="F4" s="3">
         <v>0.46188599108351125</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="15">
         <v>0.2609857505165678</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3">
         <v>6.99993E-2</v>
@@ -785,19 +754,13 @@
       <c r="F5" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="15">
         <v>1.9256810096279862</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3">
         <v>2.2911949934862328</v>
@@ -814,19 +777,13 @@
       <c r="F6" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="15">
         <v>2.907615340956998</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>0.27766422240785837</v>
@@ -843,28 +800,22 @@
       <c r="F7" s="3">
         <v>0.51275958991325354</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="15">
         <v>0.38464055555139742</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
       </c>
       <c r="E8" s="5">
         <v>1.7394000000000001</v>
@@ -872,13 +823,13 @@
       <c r="F8" s="3">
         <v>331.67023503212164</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="15">
         <v>307.19152378599557</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3">
         <v>0.35760736694113271</v>
@@ -895,13 +846,13 @@
       <c r="F9" s="3">
         <v>0.19487475215616273</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="15">
         <v>0.29727826953363679</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3">
         <v>0.42269616405056543</v>
@@ -918,13 +869,13 @@
       <c r="F10" s="3">
         <v>0.52042795266435138</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="15">
         <v>0.17493095529360692</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
         <v>0.32044600974387211</v>
@@ -941,13 +892,13 @@
       <c r="F11" s="3">
         <v>0.66550705444115821</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="15">
         <v>0.46625427737958974</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>0.74890163025752632</v>
@@ -964,19 +915,19 @@
       <c r="F12" s="3">
         <v>3.9689836546575035</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="15">
         <v>1.4211939800319573</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
       </c>
       <c r="D13" s="3">
         <v>3</v>
@@ -987,13 +938,13 @@
       <c r="F13" s="3">
         <v>117.96762389283543</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="15">
         <v>37.032230704955346</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3">
         <v>6.8579287548500317E-2</v>
@@ -1010,45 +961,45 @@
       <c r="F14" s="3">
         <v>0.08</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="3">
         <v>0.12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
       </c>
       <c r="F15" s="3">
         <v>137.64067382580706</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="15">
         <v>45.440999994429532</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
       </c>
       <c r="E16" s="5">
         <v>6.9455799999999996</v>
@@ -1056,13 +1007,13 @@
       <c r="F16" s="3">
         <v>31.61661470508102</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="15">
         <v>10.301313569938085</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.13</v>
@@ -1079,13 +1030,13 @@
       <c r="F17" s="3">
         <v>1.54</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="15">
         <v>1.1920925398944178</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3">
         <v>0.91035886781938191</v>
@@ -1102,19 +1053,19 @@
       <c r="F18" s="3">
         <v>0.95061670654940666</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <v>0.45185716699990536</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -1125,13 +1076,13 @@
       <c r="F19" s="3">
         <v>46.333491928915457</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="15">
         <v>20.483468137566732</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="3">
         <v>0.65581898788849746</v>
@@ -1148,13 +1099,13 @@
       <c r="F20" s="3">
         <v>1.0013317769081027</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="15">
         <v>0.77923128308124712</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="3">
         <v>2.5921157184870958</v>
@@ -1171,13 +1122,13 @@
       <c r="F21" s="3">
         <v>3.8704543665379876</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="15">
         <v>1.9935464335205786</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="3">
         <v>3.4666319999999994E-2</v>
@@ -1194,13 +1145,13 @@
       <c r="F22" s="3">
         <v>0.02</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="15">
         <v>1.6135813886923371</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="3">
         <v>9.333240000000001E-2</v>
@@ -1217,13 +1168,13 @@
       <c r="F23" s="3">
         <v>0.03</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="15">
         <v>3.0607146474076798</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3">
         <v>3.3095211042246296E-2</v>
@@ -1240,22 +1191,22 @@
       <c r="F24" s="3">
         <v>0.69831385476681029</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="15">
         <v>0.47034294500026319</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
       </c>
       <c r="E25" s="5">
         <v>0.87</v>
@@ -1263,13 +1214,13 @@
       <c r="F25" s="3">
         <v>2.5123016633379156</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="15">
         <v>0.28029028177023785</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="3">
         <v>0.39228594422812446</v>
@@ -1286,13 +1237,13 @@
       <c r="F26" s="3">
         <v>1.6588638034557259</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="15">
         <v>0.38390433568136328</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="3">
         <v>0.30631040232820717</v>
@@ -1309,8 +1260,56 @@
       <c r="F27" s="3">
         <v>2.7148827877877584</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="15">
         <v>2.1843886700754451</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>